<commit_message>
Added Ready Made Depth Estimation
</commit_message>
<xml_diff>
--- a/Depth/Distances.xlsx
+++ b/Depth/Distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Senior II\Graduation Project\Graduation-Project\Depth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B727C1-8560-483D-87A0-A61C8EE59DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE7DCB-1CD5-4513-99A8-98D968999BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54D01A5B-7286-4834-83CF-771D48D09616}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>Vase</t>
+  </si>
+  <si>
+    <t>Prediction using Ready Made</t>
+  </si>
+  <si>
+    <t>X using Ready Made</t>
+  </si>
+  <si>
+    <t>Depth Value Ready Made</t>
+  </si>
+  <si>
+    <t>Prediction</t>
   </si>
 </sst>
 </file>
@@ -151,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,10 +175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,7 +765,583 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.37974098562663233"/>
+                  <c:y val="-0.34974397477288083"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.78898514851485102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7420412624675501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5166835187057599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3782293806075001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8183023872679001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3596837944664002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61890199504878396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52865080023219102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2485311398354799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.68428005284015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1444954128440301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.18333333333333299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42085521380344998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4010989010988999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3388981636060099E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.44263148758895998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.80492424242424199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5037593984962401</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.20107238605898101</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.286195286195286</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.51411290322580605</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.92930029154518901</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0231923601637101</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2734400359559499</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68048389966198097</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.83876060785474604</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.61148146371876599</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.08742004264392</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.4271844660194102</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.2189349112426</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.8523489932885902</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.0147492625368697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2367-4A47-BF5F-A46463F186C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608627695"/>
+        <c:axId val="608628655"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608627695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608628655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608628655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608627695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1313,20 +1897,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>355774</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>106160</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>56763</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>146935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>46336</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66403</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>99951</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1346,6 +2446,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>416377</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>130627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>87084</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3DA3E0-0CDB-BE7D-9418-66E40732D5A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1651,10 +2787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0A81FC-E200-4595-882E-4AAB31B38124}">
-  <dimension ref="B2:J35"/>
+  <dimension ref="B2:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1665,11 +2801,14 @@
     <col min="4" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="21.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="9" width="18.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1691,8 +2830,20 @@
       <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1715,9 +2866,20 @@
       <c r="H3" s="4">
         <v>0.15779702970296999</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="4">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4">
+        <v>6.2745098039215602E-2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.78898514851485102</v>
+      </c>
+      <c r="L3" s="4">
+        <v>74.2</v>
+      </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1739,10 +2901,20 @@
       <c r="H4" s="4">
         <v>9.9764000000000005E-2</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="I4" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.101960784313725</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.7420412624675501</v>
+      </c>
+      <c r="L4" s="4">
+        <v>123.8</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1764,10 +2936,20 @@
       <c r="H5" s="4">
         <v>0.396405919661733</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="I5" s="4">
+        <v>106.6</v>
+      </c>
+      <c r="J5" s="4">
+        <v>9.0196078431372506E-2</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1.5166835187057599</v>
+      </c>
+      <c r="L5" s="4">
+        <v>114.2</v>
+      </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1789,10 +2971,20 @@
       <c r="H6" s="4">
         <v>0.244524567527137</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="I6" s="4">
+        <v>84.6</v>
+      </c>
+      <c r="J6" s="4">
+        <v>8.6274509803921498E-2</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.3782293806075001</v>
+      </c>
+      <c r="L6" s="4">
+        <v>107.6</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1814,10 +3006,21 @@
       <c r="H7" s="4">
         <v>0.73275862068965503</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="4">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="J7" s="4">
+        <v>5.0980392156862703E-2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2.8183023872679001</v>
+      </c>
+      <c r="L7" s="4">
+        <v>151.6</v>
+      </c>
+      <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1839,10 +3042,21 @@
       <c r="H8" s="4">
         <v>0.95085390409426496</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="4">
+        <v>150.80000000000001</v>
+      </c>
+      <c r="J8" s="4">
+        <v>5.8823529411764698E-2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3.3596837944664002</v>
+      </c>
+      <c r="L8" s="4">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1864,10 +3078,21 @@
       <c r="H9" s="4">
         <v>7.36138936842166E-2</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="4">
+        <v>54.6</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.105882352941176</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.61890199504878396</v>
+      </c>
+      <c r="L9" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1889,9 +3114,20 @@
       <c r="H10" s="4">
         <v>7.2194602674880801E-2</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="4">
+        <v>54.3</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.12156862745098</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.52865080023219102</v>
+      </c>
+      <c r="L10" s="4">
+        <v>56.6</v>
+      </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1913,9 +3149,20 @@
       <c r="H11" s="4">
         <v>0.42860024203307701</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="4">
+        <v>110.8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>9.0196078431372506E-2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1.2485311398354799</v>
+      </c>
+      <c r="L11" s="4">
+        <v>101</v>
+      </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1937,9 +3184,20 @@
       <c r="H12" s="4">
         <v>0.48819711676526301</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="4">
+        <v>117.9</v>
+      </c>
+      <c r="J12" s="4">
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1.68428005284015</v>
+      </c>
+      <c r="L12" s="4">
+        <v>121.5</v>
+      </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1961,9 +3219,20 @@
       <c r="H13" s="4">
         <v>0.59846383614252097</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4">
+        <v>129.4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>4.7058823529411702E-2</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.1444954128440301</v>
+      </c>
+      <c r="L13" s="4">
+        <v>137.69999999999999</v>
+      </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1985,9 +3254,20 @@
       <c r="H14" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4">
+        <v>153</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3.1372549019607801E-2</v>
+      </c>
+      <c r="K14" s="4">
+        <v>4.125</v>
+      </c>
+      <c r="L14" s="4">
+        <v>145.19999999999999</v>
+      </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -2009,9 +3289,20 @@
       <c r="H15" s="4">
         <v>5.0769230769230698E-2</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4">
+        <v>50.2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.14117647058823499</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.18333333333333299</v>
+      </c>
+      <c r="L15" s="4">
+        <v>30.5</v>
+      </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -2033,8 +3324,20 @@
       <c r="H16" s="4">
         <v>0.181201550387596</v>
       </c>
+      <c r="I16" s="4">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.12156862745098</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.42085521380344998</v>
+      </c>
+      <c r="L16" s="4">
+        <v>48.8</v>
+      </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2056,8 +3359,20 @@
       <c r="H17" s="4">
         <v>0.35470858255668303</v>
       </c>
+      <c r="I17" s="4">
+        <v>101</v>
+      </c>
+      <c r="J17" s="4">
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1.4010989010988999</v>
+      </c>
+      <c r="L17" s="4">
+        <v>108.7</v>
+      </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
@@ -2079,8 +3394,20 @@
       <c r="H18" s="4">
         <v>7.6019556403529698E-2</v>
       </c>
+      <c r="I18" s="4">
+        <v>55</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4">
+        <v>3.3388981636060099E-2</v>
+      </c>
+      <c r="L18" s="4">
+        <v>18.3</v>
+      </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
@@ -2102,8 +3429,20 @@
       <c r="H19" s="4">
         <v>0.16095690457780301</v>
       </c>
+      <c r="I19" s="4">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.10980392156862701</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.44263148758895998</v>
+      </c>
+      <c r="L19" s="4">
+        <v>50.4</v>
+      </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
@@ -2125,8 +3464,20 @@
       <c r="H20" s="4">
         <v>0.182560137457044</v>
       </c>
+      <c r="I20" s="4">
+        <v>74.3</v>
+      </c>
+      <c r="J20" s="4">
+        <v>8.6274509803921498E-2</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.80492424242424199</v>
+      </c>
+      <c r="L20" s="4">
+        <v>75.2</v>
+      </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
@@ -2148,8 +3499,20 @@
       <c r="H21" s="4">
         <v>0.36719706242349998</v>
       </c>
+      <c r="I21" s="4">
+        <v>102.7</v>
+      </c>
+      <c r="J21" s="4">
+        <v>8.2352941176470504E-2</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1.5037593984962401</v>
+      </c>
+      <c r="L21" s="4">
+        <v>113.6</v>
+      </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
@@ -2171,8 +3534,20 @@
       <c r="H22" s="4">
         <v>6.7687733920845095E-2</v>
       </c>
+      <c r="I22" s="4">
+        <v>53.4</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.20107238605898101</v>
+      </c>
+      <c r="L22" s="4">
+        <v>32</v>
+      </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>12</v>
       </c>
@@ -2194,8 +3569,20 @@
       <c r="H23" s="4">
         <v>6.0463792858158998E-2</v>
       </c>
+      <c r="I23" s="4">
+        <v>52.1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.11764705882352899</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.286195286195286</v>
+      </c>
+      <c r="L23" s="4">
+        <v>38.6</v>
+      </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
@@ -2217,8 +3604,20 @@
       <c r="H24" s="4">
         <v>0.146889400921658</v>
       </c>
+      <c r="I24" s="4">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="J24" s="4">
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.51411290322580605</v>
+      </c>
+      <c r="L24" s="4">
+        <v>55.6</v>
+      </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2240,8 +3639,20 @@
       <c r="H25" s="4">
         <v>0.14585430584789899</v>
       </c>
+      <c r="I25" s="4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.13725490196078399</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.92930029154518901</v>
+      </c>
+      <c r="L25" s="4">
+        <v>83</v>
+      </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>13</v>
       </c>
@@ -2263,8 +3674,20 @@
       <c r="H26" s="4">
         <v>0.252090871344682</v>
       </c>
+      <c r="I26" s="4">
+        <v>85.8</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1.0231923601637101</v>
+      </c>
+      <c r="L26" s="4">
+        <v>88.6</v>
+      </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
@@ -2286,8 +3709,20 @@
       <c r="H27" s="4">
         <v>0.17419698605057801</v>
       </c>
+      <c r="I27" s="4">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.113725490196078</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1.2734400359559499</v>
+      </c>
+      <c r="L27" s="4">
+        <v>102.3</v>
+      </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>14</v>
       </c>
@@ -2309,8 +3744,20 @@
       <c r="H28" s="4">
         <v>0.137345374243702</v>
       </c>
+      <c r="I28" s="4">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="J28" s="4">
+        <v>8.6274509803921498E-2</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0.68048389966198097</v>
+      </c>
+      <c r="L28" s="4">
+        <v>67.099999999999994</v>
+      </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>15</v>
       </c>
@@ -2332,8 +3779,20 @@
       <c r="H29" s="4">
         <v>0.101553974942054</v>
       </c>
+      <c r="I29" s="4">
+        <v>59.9</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.105882352941176</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0.83876060785474604</v>
+      </c>
+      <c r="L29" s="4">
+        <v>77.400000000000006</v>
+      </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>15</v>
       </c>
@@ -2355,8 +3814,20 @@
       <c r="H30" s="4">
         <v>0.106185403879306</v>
       </c>
+      <c r="I30" s="4">
+        <v>60.7</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.113725490196078</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.61148146371876599</v>
+      </c>
+      <c r="L30" s="4">
+        <v>62.4</v>
+      </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>15</v>
       </c>
@@ -2378,8 +3849,20 @@
       <c r="H31" s="4">
         <v>0.28318230277185502</v>
       </c>
+      <c r="I31" s="4">
+        <v>90.6</v>
+      </c>
+      <c r="J31" s="4">
+        <v>9.8039215686274495E-2</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1.08742004264392</v>
+      </c>
+      <c r="L31" s="4">
+        <v>92.3</v>
+      </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2401,8 +3884,20 @@
       <c r="H32" s="4">
         <v>0.51577669902912604</v>
       </c>
+      <c r="I32" s="4">
+        <v>121</v>
+      </c>
+      <c r="J32" s="4">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="K32" s="4">
+        <v>2.4271844660194102</v>
+      </c>
+      <c r="L32" s="4">
+        <v>144.9</v>
+      </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>15</v>
       </c>
@@ -2424,8 +3919,20 @@
       <c r="H33" s="4">
         <v>0.83826429980276096</v>
       </c>
+      <c r="I33" s="4">
+        <v>146.5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2.2189349112426</v>
+      </c>
+      <c r="L33" s="4">
+        <v>139.80000000000001</v>
+      </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>16</v>
       </c>
@@ -2447,8 +3954,20 @@
       <c r="H34" s="4">
         <v>0.74409104172745799</v>
       </c>
+      <c r="I34" s="4">
+        <v>141</v>
+      </c>
+      <c r="J34" s="4">
+        <v>9.41176470588235E-2</v>
+      </c>
+      <c r="K34" s="4">
+        <v>2.8523489932885902</v>
+      </c>
+      <c r="L34" s="4">
+        <v>152</v>
+      </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
         <v>16</v>
       </c>
@@ -2469,6 +3988,18 @@
       </c>
       <c r="H35" s="4">
         <v>0.90265486725663702</v>
+      </c>
+      <c r="I35" s="4">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="J35" s="4">
+        <v>7.0588235294117604E-2</v>
+      </c>
+      <c r="K35" s="4">
+        <v>5.0147492625368697</v>
+      </c>
+      <c r="L35" s="4">
+        <v>115.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>